<commit_message>
Added information for CMU (Pitt&SV), UIUC, UCLA, UCSD
</commit_message>
<xml_diff>
--- a/Program_Summary.xlsx
+++ b/Program_Summary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xuel/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xuel/Desktop/LOO/Grad_Application/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16DF988-DE8E-E944-BF4D-84C39A67E8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E48CF49-4048-074D-A129-517908E07637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15520" yWindow="740" windowWidth="14720" windowHeight="18900" activeTab="1" xr2:uid="{1693F520-B3D1-D645-ADA2-78F3A0A704D5}"/>
+    <workbookView xWindow="160" yWindow="9360" windowWidth="29920" windowHeight="8300" activeTab="1" xr2:uid="{1693F520-B3D1-D645-ADA2-78F3A0A704D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Canada" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Canada!$A$1:$I$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">US!$A$1:$J$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">US!$A$1:$K$7</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +33,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="133">
   <si>
     <t>U of T</t>
   </si>
@@ -407,9 +406,6 @@
     <t>MSML</t>
   </si>
   <si>
-    <t>MSE</t>
-  </si>
-  <si>
     <t>MSIN</t>
   </si>
   <si>
@@ -417,6 +413,49 @@
   </si>
   <si>
     <t>CMU/CMU-SV</t>
+  </si>
+  <si>
+    <t>MSECE</t>
+  </si>
+  <si>
+    <t>UCSD</t>
+  </si>
+  <si>
+    <t>GRE</t>
+  </si>
+  <si>
+    <t>Nov 19/Dec 10, 2025</t>
+  </si>
+  <si>
+    <t>Strongly Recom</t>
+  </si>
+  <si>
+    <t>https://cs.cmu.edu/academics/masters/resources/scs-masters-programs-data.xlsx</t>
+  </si>
+  <si>
+    <t>SESV</t>
+  </si>
+  <si>
+    <t>https://www.ece.cmu.edu/admissions/index.html</t>
+  </si>
+  <si>
+    <t>https://siebelschool.illinois.edu/academics/graduate/professional-mcs</t>
+  </si>
+  <si>
+    <t>https://siebelschool.illinois.edu/admissions/graduate/applications-process-requirements</t>
+  </si>
+  <si>
+    <t>https://grad.ucla.edu/programs/school-of-engineering-and-applied-science/computer-science/
+https://grad.ucla.edu/admissions/research-requirements/#Criteria</t>
+  </si>
+  <si>
+    <t>https://grad.ucla.edu/programs/school-of-engineering-and-applied-science/electrical-computer-engineering/https://grad.ucla.edu/admissions/research-requirements/#Criteria</t>
+  </si>
+  <si>
+    <t>https://cse.ucsd.edu/graduate/admissions</t>
+  </si>
+  <si>
+    <t>75(CS)/76(CE)</t>
   </si>
 </sst>
 </file>
@@ -424,7 +463,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="mmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="mmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -484,7 +523,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -497,10 +536,10 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -824,7 +863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE62A393-52B2-BF45-96CB-7720F049400F}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="90" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -1608,10 +1647,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE79B7E2-F5AB-074B-8978-53C18DCD04B8}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="G27" sqref="F25:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1620,16 +1659,17 @@
     <col min="2" max="2" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="68.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="48" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="18.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="68.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="41.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="48" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1646,22 +1686,25 @@
         <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>75</v>
       </c>
@@ -1677,23 +1720,26 @@
       <c r="E2" s="2">
         <v>45993</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>75</v>
       </c>
@@ -1709,23 +1755,26 @@
       <c r="E3" s="2">
         <v>45993</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>75</v>
       </c>
@@ -1741,23 +1790,26 @@
       <c r="E4" s="2">
         <v>45993</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>75</v>
       </c>
@@ -1773,23 +1825,26 @@
       <c r="E5" s="2">
         <v>45993</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>91</v>
       </c>
@@ -1805,20 +1860,23 @@
       <c r="E6" s="2">
         <v>45663</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>91</v>
       </c>
@@ -1834,23 +1892,26 @@
       <c r="E7" s="2">
         <v>46000</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="K7" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>91</v>
       </c>
@@ -1866,20 +1927,23 @@
       <c r="E8" s="2">
         <v>46000</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>104</v>
       </c>
@@ -1889,9 +1953,20 @@
       <c r="C9" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="E9" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>104</v>
       </c>
@@ -1901,8 +1976,11 @@
       <c r="C10" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="I10" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>104</v>
       </c>
@@ -1910,10 +1988,13 @@
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>104</v>
       </c>
@@ -1921,32 +2002,50 @@
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+      <c r="E14" s="2">
+        <v>46006</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>102</v>
       </c>
@@ -1956,8 +2055,20 @@
       <c r="C15" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="E15" s="2">
+        <v>46006</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>102</v>
       </c>
@@ -1967,63 +2078,134 @@
       <c r="C16" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="E16" s="2">
+        <v>46037</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="2">
+        <v>46006</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E18" s="2">
+        <v>46006</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E19" s="2">
+        <v>46008</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+    <row r="30" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+    <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="8" t="s">
+    <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+    <row r="33" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+    <row r="34" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+    <row r="35" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+    <row r="36" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+    <row r="37" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>112</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J7" xr:uid="{FE79B7E2-F5AB-074B-8978-53C18DCD04B8}"/>
+  <autoFilter ref="A1:K7" xr:uid="{FE79B7E2-F5AB-074B-8978-53C18DCD04B8}"/>
   <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1" display="https://ee.stanford.edu/admissions/ms" xr:uid="{BB503E17-0B8F-0C4C-9410-5BD5E1BE7E7E}"/>
-    <hyperlink ref="H6" r:id="rId2" xr:uid="{73068600-B537-B44F-B388-9A0EDFE82571}"/>
+    <hyperlink ref="I4" r:id="rId1" display="https://ee.stanford.edu/admissions/ms" xr:uid="{BB503E17-0B8F-0C4C-9410-5BD5E1BE7E7E}"/>
+    <hyperlink ref="I6" r:id="rId2" xr:uid="{73068600-B537-B44F-B388-9A0EDFE82571}"/>
+    <hyperlink ref="I17" r:id="rId3" display="https://grad.ucla.edu/programs/school-of-engineering-and-applied-science/computer-science/" xr:uid="{D0D905A7-3D0F-D544-9875-FDBADE87F7C4}"/>
+    <hyperlink ref="I18" r:id="rId4" location="Criteria" xr:uid="{8A673FC2-D2C2-134A-893F-8E7D30F00125}"/>
+    <hyperlink ref="I19" r:id="rId5" xr:uid="{016B609E-BCDF-5440-B8D9-DB6208BE395D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
UMich, GATech, UT Austin, UPenn,
</commit_message>
<xml_diff>
--- a/Program_Summary.xlsx
+++ b/Program_Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xuel/Desktop/LOO/Grad_Application/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hujitao/Desktop/master/26Fall-US-Canada-Grad-Application/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E48CF49-4048-074D-A129-517908E07637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C51667-4E5E-E241-81B1-7C78B9E6D95A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="9360" windowWidth="29920" windowHeight="8300" activeTab="1" xr2:uid="{1693F520-B3D1-D645-ADA2-78F3A0A704D5}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="21360" activeTab="1" xr2:uid="{1693F520-B3D1-D645-ADA2-78F3A0A704D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Canada" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="152">
   <si>
     <t>U of T</t>
   </si>
@@ -456,6 +456,64 @@
   </si>
   <si>
     <t>75(CS)/76(CE)</t>
+  </si>
+  <si>
+    <t>CSE</t>
+  </si>
+  <si>
+    <t>Y for undergrad outside US</t>
+  </si>
+  <si>
+    <t>https://cse.engin.umich.edu/academics/graduate/admissions/</t>
+  </si>
+  <si>
+    <t>https://ece.engin.umich.edu/academics/graduate-programs/prospective-grad-students/apply-for-grad/apply-for-meng/</t>
+  </si>
+  <si>
+    <t>GATech</t>
+  </si>
+  <si>
+    <t>MSCSE</t>
+  </si>
+  <si>
+    <t>MS Cybersecurity</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>MS ECE</t>
+  </si>
+  <si>
+    <t>Upenn</t>
+  </si>
+  <si>
+    <t>CIS</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>System Engineering</t>
+  </si>
+  <si>
+    <t>Robtics</t>
+  </si>
+  <si>
+    <t>CITMSE</t>
+  </si>
+  <si>
+    <t>https://www.cc.gatech.edu/ms-computer-science-admission-requirements</t>
+  </si>
+  <si>
+    <t>https://www.cc.gatech.edu/degree-programs/ms-computational-science-and-engineering</t>
+  </si>
+  <si>
+    <t>https://gradadm.seas.upenn.edu/faqs/do-i-need-to-take-the-gre/
+https://gradadm.seas.upenn.edu/masters/</t>
+  </si>
+  <si>
+    <t>https://www.ece.utexas.edu/academics/graduate/admissions</t>
   </si>
 </sst>
 </file>
@@ -518,7 +576,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -545,6 +603,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -565,9 +626,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -605,7 +666,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -711,7 +772,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -853,7 +914,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1647,10 +1708,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE79B7E2-F5AB-074B-8978-53C18DCD04B8}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="G27" sqref="F25:G27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2151,48 +2212,186 @@
         <v>131</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+    <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>103</v>
       </c>
+      <c r="B20" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E20" s="9">
+        <v>46037</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="9">
+        <v>45672</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="C23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="C24" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="C26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="C28" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="C29" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="30" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>105</v>
+      <c r="C30" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>108</v>
+      <c r="C31" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+    <row r="42" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2204,6 +2403,10 @@
     <hyperlink ref="I17" r:id="rId3" display="https://grad.ucla.edu/programs/school-of-engineering-and-applied-science/computer-science/" xr:uid="{D0D905A7-3D0F-D544-9875-FDBADE87F7C4}"/>
     <hyperlink ref="I18" r:id="rId4" location="Criteria" xr:uid="{8A673FC2-D2C2-134A-893F-8E7D30F00125}"/>
     <hyperlink ref="I19" r:id="rId5" xr:uid="{016B609E-BCDF-5440-B8D9-DB6208BE395D}"/>
+    <hyperlink ref="I20" r:id="rId6" xr:uid="{1CD54E77-7A83-4142-B124-3FFAD94AD195}"/>
+    <hyperlink ref="I21" r:id="rId7" xr:uid="{66982222-780D-CF40-8550-3249EBF7DA4C}"/>
+    <hyperlink ref="I23" r:id="rId8" xr:uid="{7731BD09-E158-7A47-9D8D-0D42386D4CE7}"/>
+    <hyperlink ref="I25" r:id="rId9" xr:uid="{17422755-64E4-1242-93AB-0E09A1734404}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>